<commit_message>
Feature: use cex_axis_y < 1 to make font smaller
</commit_message>
<xml_diff>
--- a/inst/extdata/james-settings.xlsx
+++ b/inst/extdata/james-settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james-package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427DF0A0-01AB-FF4D-BB48-ED4BD3C9BAD1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24488642-49E1-A64E-B413-0627CCB4D711}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12860" yWindow="4560" windowWidth="19200" windowHeight="17540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
+    <workbookView xWindow="12860" yWindow="4060" windowWidth="19200" windowHeight="17540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
   </bookViews>
   <sheets>
     <sheet name="base_settings" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>decimal_sep</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t># SCALING MARGINS</t>
+  </si>
+  <si>
+    <t>cex_axis_x</t>
+  </si>
+  <si>
+    <t>cex_axis_y</t>
   </si>
 </sst>
 </file>
@@ -478,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E64AD6-1A4D-F84C-819F-8474C164683B}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,84 +576,90 @@
         <v>6</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16">
-        <v>7.5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17">
-        <v>7.5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>7.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>7.5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <v>7</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B21">
+      <c r="B23">
         <v>-0.7</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25">
-        <v>1.8</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -655,9 +667,25 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B27">
+      <c r="B29">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Major improvements. E.g. added j_start()
</commit_message>
<xml_diff>
--- a/inst/extdata/james-settings.xlsx
+++ b/inst/extdata/james-settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james-package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34322ECA-8D32-6847-A1E4-14EC60493F6F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BF9C4D-949B-7F45-ACD8-4E2ECCF39CC1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12880" yWindow="2260" windowWidth="19200" windowHeight="17540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
   </bookViews>
@@ -339,21 +339,12 @@
     <t>dir_png</t>
   </si>
   <si>
-    <t>pdf</t>
-  </si>
-  <si>
-    <t>png</t>
-  </si>
-  <si>
     <t>color of the mark (x)</t>
   </si>
   <si>
     <t>dir_input</t>
   </si>
   <si>
-    <t>.</t>
-  </si>
-  <si>
     <t>default directories (are created if non-existent)</t>
   </si>
   <si>
@@ -412,6 +403,15 @@
   </si>
   <si>
     <t>col_bg</t>
+  </si>
+  <si>
+    <t>pdf/</t>
+  </si>
+  <si>
+    <t>png/</t>
+  </si>
+  <si>
+    <t>./</t>
   </si>
 </sst>
 </file>
@@ -793,7 +793,7 @@
   <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -819,25 +819,25 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -846,7 +846,7 @@
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -854,7 +854,7 @@
         <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -864,7 +864,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
         <v>87</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
         <v>86</v>
@@ -908,18 +908,18 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s">
         <v>98</v>
@@ -927,13 +927,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
         <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1044,21 +1044,21 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B30">
         <v>0.02</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D30" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1454,23 +1454,23 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B81" t="s">
+        <v>113</v>
+      </c>
+      <c r="C81" t="s">
         <v>116</v>
-      </c>
-      <c r="C81" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B82">
         <v>2400</v>

</xml_diff>

<commit_message>
New colors for bg and future
</commit_message>
<xml_diff>
--- a/inst/extdata/james-settings.xlsx
+++ b/inst/extdata/james-settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james-package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDDAF25-676D-AD49-BD0E-EE6281814638}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5062EABB-462F-9645-AE63-305D52649057}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12880" yWindow="2260" windowWidth="19200" windowHeight="17540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
   </bookViews>
@@ -126,9 +126,6 @@
     <t>#000000</t>
   </si>
   <si>
-    <t>#eeeeee</t>
-  </si>
-  <si>
     <t>lwd_help_lines</t>
   </si>
   <si>
@@ -285,9 +282,6 @@
     <t>#0071bb, #7dcef1, #ed0579, #fbd4dc, #95817b, #00aeef, #003f71, #7b0052</t>
   </si>
   <si>
-    <t>#e4f5fd</t>
-  </si>
-  <si>
     <t>background color</t>
   </si>
   <si>
@@ -421,6 +415,12 @@
   </si>
   <si>
     <t>#FFFFFF, #FF0000</t>
+  </si>
+  <si>
+    <t>#eef8ff</t>
+  </si>
+  <si>
+    <t>#ffffff</t>
   </si>
 </sst>
 </file>
@@ -802,7 +802,7 @@
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -817,53 +817,53 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -873,21 +873,21 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -895,65 +895,65 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
         <v>97</v>
-      </c>
-      <c r="C11" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" t="s">
         <v>120</v>
-      </c>
-      <c r="B12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" t="s">
         <v>129</v>
       </c>
-      <c r="B13" t="s">
-        <v>131</v>
-      </c>
       <c r="C13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -961,7 +961,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -969,7 +969,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
         <v>32</v>
@@ -977,13 +977,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1015,13 +1015,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>2</v>
@@ -1051,12 +1051,12 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1064,21 +1064,21 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B31">
         <v>0.02</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1099,7 +1099,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>0.25</v>
@@ -1118,24 +1118,24 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1151,23 +1151,23 @@
         <v>0.4</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B44">
         <v>0.4</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1177,16 +1177,16 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1202,21 +1202,21 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B49">
         <v>0.02</v>
       </c>
       <c r="C49" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D49" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B50">
         <v>0.25</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B51">
         <v>-1.4999999999999999E-2</v>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B56">
         <v>21</v>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B57">
         <v>21</v>
@@ -1292,114 +1292,114 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" t="s">
         <v>83</v>
-      </c>
-      <c r="C61" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62">
         <v>0.5</v>
       </c>
       <c r="C62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>0.5</v>
       </c>
       <c r="C63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B64">
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B65">
         <v>0.5</v>
       </c>
       <c r="C65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B67">
         <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68">
         <v>0.03</v>
       </c>
       <c r="C68" t="s">
+        <v>79</v>
+      </c>
+      <c r="D68" t="s">
         <v>80</v>
-      </c>
-      <c r="D68" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B69">
         <v>0.12</v>
       </c>
       <c r="D69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1410,7 +1410,7 @@
         <v>0.6</v>
       </c>
       <c r="C72" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1439,18 +1439,18 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B76">
         <v>0</v>
       </c>
       <c r="C76" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B77">
         <v>1.5</v>
@@ -1458,7 +1458,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -1466,7 +1466,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -1474,23 +1474,23 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B82" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C82" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B83">
         <v>2400</v>

</xml_diff>

<commit_message>
color gradient in legend heatmap
</commit_message>
<xml_diff>
--- a/inst/extdata/james-settings.xlsx
+++ b/inst/extdata/james-settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james-package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5062EABB-462F-9645-AE63-305D52649057}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F832B7C0-CB61-B249-8B12-A54556891C9A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12880" yWindow="2260" windowWidth="19200" windowHeight="17540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
   </bookViews>
@@ -414,13 +414,13 @@
     <t>low to high</t>
   </si>
   <si>
-    <t>#FFFFFF, #FF0000</t>
-  </si>
-  <si>
     <t>#eef8ff</t>
   </si>
   <si>
     <t>#ffffff</t>
+  </si>
+  <si>
+    <t>white, red</t>
   </si>
 </sst>
 </file>
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E64AD6-1A4D-F84C-819F-8474C164683B}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -876,7 +876,7 @@
         <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" t="s">
         <v>85</v>
@@ -931,7 +931,7 @@
         <v>127</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C13" t="s">
         <v>128</v>
@@ -961,7 +961,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Added paramter to lift x_lab
</commit_message>
<xml_diff>
--- a/inst/extdata/james-settings.xlsx
+++ b/inst/extdata/james-settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james-package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F832B7C0-CB61-B249-8B12-A54556891C9A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81CEC04-BFCE-8E4F-99CE-63281B356785}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12880" yWindow="2260" windowWidth="19200" windowHeight="17540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="134">
   <si>
     <t>decimal_sep</t>
   </si>
@@ -421,6 +421,12 @@
   </si>
   <si>
     <t>white, red</t>
+  </si>
+  <si>
+    <t>v_shift_x_lab</t>
+  </si>
+  <si>
+    <t>shift x_lab down (+1 means one line lower)</t>
   </si>
 </sst>
 </file>
@@ -799,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E64AD6-1A4D-F84C-819F-8474C164683B}">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1230,25 +1236,25 @@
         <v>-1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52">
+        <v>0.9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>3</v>
-      </c>
-      <c r="B54">
-        <v>7.5</v>
-      </c>
-      <c r="D54" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B55">
         <v>7.5</v>
@@ -1259,10 +1265,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="B56">
-        <v>21</v>
+        <v>7.5</v>
       </c>
       <c r="D56" t="s">
         <v>4</v>
@@ -1270,7 +1276,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B57">
         <v>21</v>
@@ -1281,149 +1287,152 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58">
+        <v>21</v>
+      </c>
+      <c r="D58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>10</v>
       </c>
-      <c r="B58">
+      <c r="B59">
         <v>7</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>59</v>
-      </c>
-      <c r="B62">
-        <v>0.5</v>
-      </c>
-      <c r="C62" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B63">
         <v>0.5</v>
       </c>
       <c r="C63" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="C64" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B65">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C66" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="B67">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>71</v>
-      </c>
-      <c r="D67" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B68">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D68" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69">
+        <v>0.03</v>
+      </c>
+      <c r="C69" t="s">
+        <v>79</v>
+      </c>
+      <c r="D69" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>78</v>
       </c>
-      <c r="B69">
+      <c r="B70">
         <v>0.12</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D70" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>21</v>
-      </c>
-      <c r="B72">
-        <v>0.6</v>
-      </c>
-      <c r="C72" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B73">
-        <v>0.5</v>
+        <v>0.6</v>
+      </c>
+      <c r="C73" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B74">
         <v>0.5</v>
@@ -1431,68 +1440,76 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B75">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B76">
-        <v>0</v>
-      </c>
-      <c r="C76" t="s">
-        <v>46</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B77">
-        <v>1.5</v>
+        <v>0</v>
+      </c>
+      <c r="C77" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>42</v>
       </c>
-      <c r="B79">
+      <c r="B80">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>112</v>
-      </c>
-      <c r="B82" t="s">
-        <v>110</v>
-      </c>
-      <c r="C82" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>112</v>
+      </c>
+      <c r="B83" t="s">
+        <v>110</v>
+      </c>
+      <c r="C83" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>111</v>
       </c>
-      <c r="B83">
+      <c r="B84">
         <v>2400</v>
       </c>
     </row>

</xml_diff>